<commit_message>
Add function to create regular berb form change.
</commit_message>
<xml_diff>
--- a/Verbs.xlsx
+++ b/Verbs.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23120"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{490F91C3-F87E-48F3-8630-8D0E9A574526}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{13999442-B72B-41C2-BCD3-ADCE95037647}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,21 +25,39 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
-  <si>
-    <t>Yo</t>
-  </si>
-  <si>
-    <t>Vos</t>
-  </si>
-  <si>
-    <t>El/Ella/Usted</t>
-  </si>
-  <si>
-    <t>Nosotros/Nosotras</t>
-  </si>
-  <si>
-    <t>Ellos/Ellas/Ustedes</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="196">
+  <si>
+    <t>yo</t>
+  </si>
+  <si>
+    <t>vos</t>
+  </si>
+  <si>
+    <t>el/ella/usted</t>
+  </si>
+  <si>
+    <t>nosotros/nosotras</t>
+  </si>
+  <si>
+    <t>ellos/ellas/ustedes</t>
+  </si>
+  <si>
+    <t>hablar</t>
+  </si>
+  <si>
+    <t>hablo</t>
+  </si>
+  <si>
+    <t>hablás</t>
+  </si>
+  <si>
+    <t>habla</t>
+  </si>
+  <si>
+    <t>hablamos</t>
+  </si>
+  <si>
+    <t>hablan</t>
   </si>
   <si>
     <t>comer</t>
@@ -58,6 +76,543 @@
   </si>
   <si>
     <t>comen</t>
+  </si>
+  <si>
+    <t>vivir</t>
+  </si>
+  <si>
+    <t>vivo</t>
+  </si>
+  <si>
+    <t>vivís</t>
+  </si>
+  <si>
+    <t>vive</t>
+  </si>
+  <si>
+    <t>vivimos</t>
+  </si>
+  <si>
+    <t>viven</t>
+  </si>
+  <si>
+    <t>ser</t>
+  </si>
+  <si>
+    <t>soy</t>
+  </si>
+  <si>
+    <t>sos</t>
+  </si>
+  <si>
+    <t>es</t>
+  </si>
+  <si>
+    <t>somos</t>
+  </si>
+  <si>
+    <t>son</t>
+  </si>
+  <si>
+    <t>ir</t>
+  </si>
+  <si>
+    <t>voy</t>
+  </si>
+  <si>
+    <t>vas</t>
+  </si>
+  <si>
+    <t>va</t>
+  </si>
+  <si>
+    <t>vamos</t>
+  </si>
+  <si>
+    <t>van</t>
+  </si>
+  <si>
+    <t>estar</t>
+  </si>
+  <si>
+    <t>estoy</t>
+  </si>
+  <si>
+    <t>estás</t>
+  </si>
+  <si>
+    <t>está</t>
+  </si>
+  <si>
+    <t>estamos</t>
+  </si>
+  <si>
+    <t>están</t>
+  </si>
+  <si>
+    <t>dar</t>
+  </si>
+  <si>
+    <t>doy</t>
+  </si>
+  <si>
+    <t>das</t>
+  </si>
+  <si>
+    <t>da</t>
+  </si>
+  <si>
+    <t>damos</t>
+  </si>
+  <si>
+    <t>dan</t>
+  </si>
+  <si>
+    <t>conocer</t>
+  </si>
+  <si>
+    <t>conozco</t>
+  </si>
+  <si>
+    <t>conocés</t>
+  </si>
+  <si>
+    <t>conoce</t>
+  </si>
+  <si>
+    <t>conocemos</t>
+  </si>
+  <si>
+    <t>conocen</t>
+  </si>
+  <si>
+    <t>ofrecer</t>
+  </si>
+  <si>
+    <t>ofrezco</t>
+  </si>
+  <si>
+    <t>ofrecés</t>
+  </si>
+  <si>
+    <t>ofrece</t>
+  </si>
+  <si>
+    <t>ofrecemos</t>
+  </si>
+  <si>
+    <t>ofrecen</t>
+  </si>
+  <si>
+    <t>hacer</t>
+  </si>
+  <si>
+    <t>hago</t>
+  </si>
+  <si>
+    <t>hacés</t>
+  </si>
+  <si>
+    <t>hace</t>
+  </si>
+  <si>
+    <t>hacemos</t>
+  </si>
+  <si>
+    <t>hacen</t>
+  </si>
+  <si>
+    <t>salir</t>
+  </si>
+  <si>
+    <t>salgo</t>
+  </si>
+  <si>
+    <t>salís</t>
+  </si>
+  <si>
+    <t>sale</t>
+  </si>
+  <si>
+    <t>salimos</t>
+  </si>
+  <si>
+    <t>salen</t>
+  </si>
+  <si>
+    <t>querer</t>
+  </si>
+  <si>
+    <t>quiero</t>
+  </si>
+  <si>
+    <t>querés</t>
+  </si>
+  <si>
+    <t>quiere</t>
+  </si>
+  <si>
+    <t>queremos</t>
+  </si>
+  <si>
+    <t>quieren</t>
+  </si>
+  <si>
+    <t>empezar</t>
+  </si>
+  <si>
+    <t>empiezo</t>
+  </si>
+  <si>
+    <t>empezás</t>
+  </si>
+  <si>
+    <t>empieza</t>
+  </si>
+  <si>
+    <t>empezamos</t>
+  </si>
+  <si>
+    <t>empiezan</t>
+  </si>
+  <si>
+    <t>despertarse</t>
+  </si>
+  <si>
+    <t>me despierto</t>
+  </si>
+  <si>
+    <t>te despertás</t>
+  </si>
+  <si>
+    <t>se despierta</t>
+  </si>
+  <si>
+    <t>nos despertamos</t>
+  </si>
+  <si>
+    <t>se despiertan</t>
+  </si>
+  <si>
+    <t>sentir</t>
+  </si>
+  <si>
+    <t>siento</t>
+  </si>
+  <si>
+    <t>sentís</t>
+  </si>
+  <si>
+    <t>siente</t>
+  </si>
+  <si>
+    <t>sentimos</t>
+  </si>
+  <si>
+    <t>sienten</t>
+  </si>
+  <si>
+    <t>entender</t>
+  </si>
+  <si>
+    <t>entiendo</t>
+  </si>
+  <si>
+    <t>entendés</t>
+  </si>
+  <si>
+    <t>entiende</t>
+  </si>
+  <si>
+    <t>entendemos</t>
+  </si>
+  <si>
+    <t>entienden</t>
+  </si>
+  <si>
+    <t>pensar</t>
+  </si>
+  <si>
+    <t>pienso</t>
+  </si>
+  <si>
+    <t>pensás</t>
+  </si>
+  <si>
+    <t>piensa</t>
+  </si>
+  <si>
+    <t>pensamos</t>
+  </si>
+  <si>
+    <t>piensan</t>
+  </si>
+  <si>
+    <t>pedir</t>
+  </si>
+  <si>
+    <t>pido</t>
+  </si>
+  <si>
+    <t>pedís</t>
+  </si>
+  <si>
+    <t>pide</t>
+  </si>
+  <si>
+    <t>pedimos</t>
+  </si>
+  <si>
+    <t>piden</t>
+  </si>
+  <si>
+    <t>vestirse</t>
+  </si>
+  <si>
+    <t>me visto</t>
+  </si>
+  <si>
+    <t>te vestís</t>
+  </si>
+  <si>
+    <t>se viste</t>
+  </si>
+  <si>
+    <t>nos vestimos</t>
+  </si>
+  <si>
+    <t>se visten</t>
+  </si>
+  <si>
+    <t>medir</t>
+  </si>
+  <si>
+    <t>mido</t>
+  </si>
+  <si>
+    <t>medís</t>
+  </si>
+  <si>
+    <t>mide</t>
+  </si>
+  <si>
+    <t>medimos</t>
+  </si>
+  <si>
+    <t>miden</t>
+  </si>
+  <si>
+    <t>elegir</t>
+  </si>
+  <si>
+    <t>elijo</t>
+  </si>
+  <si>
+    <t>elegís</t>
+  </si>
+  <si>
+    <t>elige</t>
+  </si>
+  <si>
+    <t>elegimos</t>
+  </si>
+  <si>
+    <t>eligen</t>
+  </si>
+  <si>
+    <t>seguir</t>
+  </si>
+  <si>
+    <t>sigo</t>
+  </si>
+  <si>
+    <t>seguís</t>
+  </si>
+  <si>
+    <t>sigue</t>
+  </si>
+  <si>
+    <t>seguimos</t>
+  </si>
+  <si>
+    <t>siguen</t>
+  </si>
+  <si>
+    <t>volver</t>
+  </si>
+  <si>
+    <t>vuelvo</t>
+  </si>
+  <si>
+    <t>volvés</t>
+  </si>
+  <si>
+    <t>vuelve</t>
+  </si>
+  <si>
+    <t>volvemos</t>
+  </si>
+  <si>
+    <t>vuelven</t>
+  </si>
+  <si>
+    <t>dormir</t>
+  </si>
+  <si>
+    <t>duermo</t>
+  </si>
+  <si>
+    <t>dormís</t>
+  </si>
+  <si>
+    <t>duerme</t>
+  </si>
+  <si>
+    <t>dormimos</t>
+  </si>
+  <si>
+    <t>duermen</t>
+  </si>
+  <si>
+    <t>acostarse</t>
+  </si>
+  <si>
+    <t>me acuesto</t>
+  </si>
+  <si>
+    <t>te acostás</t>
+  </si>
+  <si>
+    <t>se acuesta</t>
+  </si>
+  <si>
+    <t>nos acostamos</t>
+  </si>
+  <si>
+    <t>se acuestan</t>
+  </si>
+  <si>
+    <t>almorzar</t>
+  </si>
+  <si>
+    <t>almuerzo</t>
+  </si>
+  <si>
+    <t>almorzás</t>
+  </si>
+  <si>
+    <t>almuerza</t>
+  </si>
+  <si>
+    <t>almorzamos</t>
+  </si>
+  <si>
+    <t>almuerzan</t>
+  </si>
+  <si>
+    <t>costar</t>
+  </si>
+  <si>
+    <t>cuesto</t>
+  </si>
+  <si>
+    <t>costás</t>
+  </si>
+  <si>
+    <t>cuesta</t>
+  </si>
+  <si>
+    <t>costamos</t>
+  </si>
+  <si>
+    <t>cuestan</t>
+  </si>
+  <si>
+    <t>contar</t>
+  </si>
+  <si>
+    <t>cuento</t>
+  </si>
+  <si>
+    <t>contás</t>
+  </si>
+  <si>
+    <t>cuenta</t>
+  </si>
+  <si>
+    <t>contamos</t>
+  </si>
+  <si>
+    <t>cuentan</t>
+  </si>
+  <si>
+    <t>jugar</t>
+  </si>
+  <si>
+    <t>juego</t>
+  </si>
+  <si>
+    <t>jugás</t>
+  </si>
+  <si>
+    <t>juega</t>
+  </si>
+  <si>
+    <t>jugamos</t>
+  </si>
+  <si>
+    <t>juegan</t>
+  </si>
+  <si>
+    <t>llamarse</t>
+  </si>
+  <si>
+    <t>estudiar</t>
+  </si>
+  <si>
+    <t>bailar</t>
+  </si>
+  <si>
+    <t>recibir</t>
+  </si>
+  <si>
+    <t>desayunar</t>
+  </si>
+  <si>
+    <t>beber</t>
+  </si>
+  <si>
+    <t>usar</t>
+  </si>
+  <si>
+    <t>pasear</t>
+  </si>
+  <si>
+    <t>deber</t>
+  </si>
+  <si>
+    <t>practicar</t>
+  </si>
+  <si>
+    <t>subir</t>
+  </si>
+  <si>
+    <t>comprar</t>
+  </si>
+  <si>
+    <t>aprender</t>
+  </si>
+  <si>
+    <t>caminar</t>
+  </si>
+  <si>
+    <t>nadar</t>
+  </si>
+  <si>
+    <t>tocar</t>
+  </si>
+  <si>
+    <t>imprimir</t>
   </si>
 </sst>
 </file>
@@ -409,14 +964,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:F47"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
+      <selection activeCell="A48" sqref="A48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
+    <col min="1" max="1" width="11.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="4" width="15.7109375" customWidth="1"/>
     <col min="5" max="5" width="18.140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="18.42578125" bestFit="1" customWidth="1"/>
@@ -459,6 +1015,651 @@
         <v>10</v>
       </c>
     </row>
+    <row r="3" spans="1:6">
+      <c r="A3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4" t="s">
+        <v>20</v>
+      </c>
+      <c r="E4" t="s">
+        <v>21</v>
+      </c>
+      <c r="F4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D5" t="s">
+        <v>26</v>
+      </c>
+      <c r="E5" t="s">
+        <v>27</v>
+      </c>
+      <c r="F5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" t="s">
+        <v>29</v>
+      </c>
+      <c r="B6" t="s">
+        <v>30</v>
+      </c>
+      <c r="C6" t="s">
+        <v>31</v>
+      </c>
+      <c r="D6" t="s">
+        <v>32</v>
+      </c>
+      <c r="E6" t="s">
+        <v>33</v>
+      </c>
+      <c r="F6" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" t="s">
+        <v>35</v>
+      </c>
+      <c r="B7" t="s">
+        <v>36</v>
+      </c>
+      <c r="C7" t="s">
+        <v>37</v>
+      </c>
+      <c r="D7" t="s">
+        <v>38</v>
+      </c>
+      <c r="E7" t="s">
+        <v>39</v>
+      </c>
+      <c r="F7" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" t="s">
+        <v>41</v>
+      </c>
+      <c r="B8" t="s">
+        <v>42</v>
+      </c>
+      <c r="C8" t="s">
+        <v>43</v>
+      </c>
+      <c r="D8" t="s">
+        <v>44</v>
+      </c>
+      <c r="E8" t="s">
+        <v>45</v>
+      </c>
+      <c r="F8" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" t="s">
+        <v>47</v>
+      </c>
+      <c r="B9" t="s">
+        <v>48</v>
+      </c>
+      <c r="C9" t="s">
+        <v>49</v>
+      </c>
+      <c r="D9" t="s">
+        <v>50</v>
+      </c>
+      <c r="E9" t="s">
+        <v>51</v>
+      </c>
+      <c r="F9" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" t="s">
+        <v>53</v>
+      </c>
+      <c r="B10" t="s">
+        <v>54</v>
+      </c>
+      <c r="C10" t="s">
+        <v>55</v>
+      </c>
+      <c r="D10" t="s">
+        <v>56</v>
+      </c>
+      <c r="E10" t="s">
+        <v>57</v>
+      </c>
+      <c r="F10" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" t="s">
+        <v>59</v>
+      </c>
+      <c r="B11" t="s">
+        <v>60</v>
+      </c>
+      <c r="C11" t="s">
+        <v>61</v>
+      </c>
+      <c r="D11" t="s">
+        <v>62</v>
+      </c>
+      <c r="E11" t="s">
+        <v>63</v>
+      </c>
+      <c r="F11" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12" t="s">
+        <v>65</v>
+      </c>
+      <c r="B12" t="s">
+        <v>66</v>
+      </c>
+      <c r="C12" t="s">
+        <v>67</v>
+      </c>
+      <c r="D12" t="s">
+        <v>68</v>
+      </c>
+      <c r="E12" t="s">
+        <v>69</v>
+      </c>
+      <c r="F12" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13" t="s">
+        <v>71</v>
+      </c>
+      <c r="B13" t="s">
+        <v>72</v>
+      </c>
+      <c r="C13" t="s">
+        <v>73</v>
+      </c>
+      <c r="D13" t="s">
+        <v>74</v>
+      </c>
+      <c r="E13" t="s">
+        <v>75</v>
+      </c>
+      <c r="F13" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14" t="s">
+        <v>77</v>
+      </c>
+      <c r="B14" t="s">
+        <v>78</v>
+      </c>
+      <c r="C14" t="s">
+        <v>79</v>
+      </c>
+      <c r="D14" t="s">
+        <v>80</v>
+      </c>
+      <c r="E14" t="s">
+        <v>81</v>
+      </c>
+      <c r="F14" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15" t="s">
+        <v>83</v>
+      </c>
+      <c r="B15" t="s">
+        <v>84</v>
+      </c>
+      <c r="C15" t="s">
+        <v>85</v>
+      </c>
+      <c r="D15" t="s">
+        <v>86</v>
+      </c>
+      <c r="E15" t="s">
+        <v>87</v>
+      </c>
+      <c r="F15" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16" t="s">
+        <v>89</v>
+      </c>
+      <c r="B16" t="s">
+        <v>90</v>
+      </c>
+      <c r="C16" t="s">
+        <v>91</v>
+      </c>
+      <c r="D16" t="s">
+        <v>92</v>
+      </c>
+      <c r="E16" t="s">
+        <v>93</v>
+      </c>
+      <c r="F16" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
+      <c r="A17" t="s">
+        <v>95</v>
+      </c>
+      <c r="B17" t="s">
+        <v>96</v>
+      </c>
+      <c r="C17" t="s">
+        <v>97</v>
+      </c>
+      <c r="D17" t="s">
+        <v>98</v>
+      </c>
+      <c r="E17" t="s">
+        <v>99</v>
+      </c>
+      <c r="F17" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
+      <c r="A18" t="s">
+        <v>101</v>
+      </c>
+      <c r="B18" t="s">
+        <v>102</v>
+      </c>
+      <c r="C18" t="s">
+        <v>103</v>
+      </c>
+      <c r="D18" t="s">
+        <v>104</v>
+      </c>
+      <c r="E18" t="s">
+        <v>105</v>
+      </c>
+      <c r="F18" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
+      <c r="A19" t="s">
+        <v>107</v>
+      </c>
+      <c r="B19" t="s">
+        <v>108</v>
+      </c>
+      <c r="C19" t="s">
+        <v>109</v>
+      </c>
+      <c r="D19" t="s">
+        <v>110</v>
+      </c>
+      <c r="E19" t="s">
+        <v>111</v>
+      </c>
+      <c r="F19" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
+      <c r="A20" t="s">
+        <v>113</v>
+      </c>
+      <c r="B20" t="s">
+        <v>114</v>
+      </c>
+      <c r="C20" t="s">
+        <v>115</v>
+      </c>
+      <c r="D20" t="s">
+        <v>116</v>
+      </c>
+      <c r="E20" t="s">
+        <v>117</v>
+      </c>
+      <c r="F20" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6">
+      <c r="A21" t="s">
+        <v>119</v>
+      </c>
+      <c r="B21" t="s">
+        <v>120</v>
+      </c>
+      <c r="C21" t="s">
+        <v>121</v>
+      </c>
+      <c r="D21" t="s">
+        <v>122</v>
+      </c>
+      <c r="E21" t="s">
+        <v>123</v>
+      </c>
+      <c r="F21" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6">
+      <c r="A22" t="s">
+        <v>125</v>
+      </c>
+      <c r="B22" t="s">
+        <v>126</v>
+      </c>
+      <c r="C22" t="s">
+        <v>127</v>
+      </c>
+      <c r="D22" t="s">
+        <v>128</v>
+      </c>
+      <c r="E22" t="s">
+        <v>129</v>
+      </c>
+      <c r="F22" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6">
+      <c r="A23" t="s">
+        <v>131</v>
+      </c>
+      <c r="B23" t="s">
+        <v>132</v>
+      </c>
+      <c r="C23" t="s">
+        <v>133</v>
+      </c>
+      <c r="D23" t="s">
+        <v>134</v>
+      </c>
+      <c r="E23" t="s">
+        <v>135</v>
+      </c>
+      <c r="F23" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6">
+      <c r="A24" t="s">
+        <v>137</v>
+      </c>
+      <c r="B24" t="s">
+        <v>138</v>
+      </c>
+      <c r="C24" t="s">
+        <v>139</v>
+      </c>
+      <c r="D24" t="s">
+        <v>140</v>
+      </c>
+      <c r="E24" t="s">
+        <v>141</v>
+      </c>
+      <c r="F24" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6">
+      <c r="A25" t="s">
+        <v>143</v>
+      </c>
+      <c r="B25" t="s">
+        <v>144</v>
+      </c>
+      <c r="C25" t="s">
+        <v>145</v>
+      </c>
+      <c r="D25" t="s">
+        <v>146</v>
+      </c>
+      <c r="E25" t="s">
+        <v>147</v>
+      </c>
+      <c r="F25" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6">
+      <c r="A26" t="s">
+        <v>149</v>
+      </c>
+      <c r="B26" t="s">
+        <v>150</v>
+      </c>
+      <c r="C26" t="s">
+        <v>151</v>
+      </c>
+      <c r="D26" t="s">
+        <v>152</v>
+      </c>
+      <c r="E26" t="s">
+        <v>153</v>
+      </c>
+      <c r="F26" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6">
+      <c r="A27" t="s">
+        <v>155</v>
+      </c>
+      <c r="B27" t="s">
+        <v>156</v>
+      </c>
+      <c r="C27" t="s">
+        <v>157</v>
+      </c>
+      <c r="D27" t="s">
+        <v>158</v>
+      </c>
+      <c r="E27" t="s">
+        <v>159</v>
+      </c>
+      <c r="F27" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6">
+      <c r="A28" t="s">
+        <v>161</v>
+      </c>
+      <c r="B28" t="s">
+        <v>162</v>
+      </c>
+      <c r="C28" t="s">
+        <v>163</v>
+      </c>
+      <c r="D28" t="s">
+        <v>164</v>
+      </c>
+      <c r="E28" t="s">
+        <v>165</v>
+      </c>
+      <c r="F28" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6">
+      <c r="A29" t="s">
+        <v>167</v>
+      </c>
+      <c r="B29" t="s">
+        <v>168</v>
+      </c>
+      <c r="C29" t="s">
+        <v>169</v>
+      </c>
+      <c r="D29" t="s">
+        <v>170</v>
+      </c>
+      <c r="E29" t="s">
+        <v>171</v>
+      </c>
+      <c r="F29" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6">
+      <c r="A30" t="s">
+        <v>173</v>
+      </c>
+      <c r="B30" t="s">
+        <v>174</v>
+      </c>
+      <c r="C30" t="s">
+        <v>175</v>
+      </c>
+      <c r="D30" t="s">
+        <v>176</v>
+      </c>
+      <c r="E30" t="s">
+        <v>177</v>
+      </c>
+      <c r="F30" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6">
+      <c r="A31" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6">
+      <c r="A32" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1">
+      <c r="A33" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1">
+      <c r="A34" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1">
+      <c r="A35" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1">
+      <c r="A36" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1">
+      <c r="A37" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1">
+      <c r="A38" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1">
+      <c r="A39" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1">
+      <c r="A40" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1">
+      <c r="A41" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1">
+      <c r="A42" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1">
+      <c r="A43" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1">
+      <c r="A44" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1">
+      <c r="A45" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1">
+      <c r="A46" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1">
+      <c r="A47" t="s">
+        <v>195</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>